<commit_message>
Committed validations in personalise page
</commit_message>
<xml_diff>
--- a/test/integration/TestAccs.xlsx
+++ b/test/integration/TestAccs.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davuluris\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12990" windowHeight="2520"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="Status" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M17"/>
 </workbook>
 </file>
 
@@ -47,7 +51,7 @@
     <t>20150914006</t>
   </si>
   <si>
-    <t>20150914007</t>
+    <t>20150914005</t>
   </si>
 </sst>
 </file>
@@ -393,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +409,7 @@
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -428,9 +432,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -451,9 +455,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -474,39 +478,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
do personalise locator fix
</commit_message>
<xml_diff>
--- a/test/integration/TestAccs.xlsx
+++ b/test/integration/TestAccs.xlsx
@@ -44,10 +44,10 @@
     <t>Username</t>
   </si>
   <si>
-    <t>20150914011</t>
-  </si>
-  <si>
-    <t>20150914012</t>
+    <t>20150914015</t>
+  </si>
+  <si>
+    <t>20150914016</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>